<commit_message>
choosen golden truth for htr
</commit_message>
<xml_diff>
--- a/data/index/corpus_a_index.xlsx
+++ b/data/index/corpus_a_index.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eugenia/Desktop/thesis/magic_tagger/data/index/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BB3D47C-1279-7349-850D-5B442BE7EBB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD0F1A6-B6FF-2745-876F-7C5D32099531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="18360" xr2:uid="{2FED5107-BDBA-42C2-8B25-B9C3018C5C1C}"/>
+    <workbookView xWindow="10480" yWindow="1660" windowWidth="29400" windowHeight="18360" xr2:uid="{2FED5107-BDBA-42C2-8B25-B9C3018C5C1C}"/>
   </bookViews>
   <sheets>
     <sheet name="veneime13102025" sheetId="1" r:id="rId1"/>
@@ -3286,11 +3286,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B84DAE8B-405E-4655-89DF-BEE99C6D5E84}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AC118"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A31" sqref="A31:AC31"/>
+      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3414,7 +3415,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:29" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>498</v>
       </c>
@@ -3475,7 +3476,7 @@
       <c r="AB2" s="1"/>
       <c r="AC2" s="11"/>
     </row>
-    <row r="3" spans="1:29" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:29" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>499</v>
       </c>
@@ -3540,7 +3541,7 @@
       <c r="AB3" s="1"/>
       <c r="AC3" s="11"/>
     </row>
-    <row r="4" spans="1:29" ht="256" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:29" ht="256" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>500</v>
       </c>
@@ -3601,7 +3602,7 @@
       <c r="AB4" s="1"/>
       <c r="AC4" s="11"/>
     </row>
-    <row r="5" spans="1:29" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:29" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>501</v>
       </c>
@@ -3660,7 +3661,7 @@
       <c r="AB5" s="1"/>
       <c r="AC5" s="11"/>
     </row>
-    <row r="6" spans="1:29" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:29" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>502</v>
       </c>
@@ -3721,7 +3722,7 @@
       <c r="AB6" s="1"/>
       <c r="AC6" s="11"/>
     </row>
-    <row r="7" spans="1:29" ht="144" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:29" ht="144" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>503</v>
       </c>
@@ -3782,7 +3783,7 @@
       <c r="AB7" s="1"/>
       <c r="AC7" s="11"/>
     </row>
-    <row r="8" spans="1:29" ht="80" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:29" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>504</v>
       </c>
@@ -3843,7 +3844,7 @@
       <c r="AB8" s="1"/>
       <c r="AC8" s="11"/>
     </row>
-    <row r="9" spans="1:29" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:29" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>506</v>
       </c>
@@ -3910,7 +3911,7 @@
       <c r="AB9" s="1"/>
       <c r="AC9" s="11"/>
     </row>
-    <row r="10" spans="1:29" ht="64" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:29" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>507</v>
       </c>
@@ -3975,7 +3976,7 @@
       <c r="AB10" s="1"/>
       <c r="AC10" s="11"/>
     </row>
-    <row r="11" spans="1:29" ht="112" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:29" ht="112" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>508</v>
       </c>
@@ -4032,7 +4033,7 @@
       <c r="AB11" s="1"/>
       <c r="AC11" s="11"/>
     </row>
-    <row r="12" spans="1:29" ht="144" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:29" ht="144" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>519</v>
       </c>
@@ -4091,7 +4092,7 @@
       <c r="AB12" s="1"/>
       <c r="AC12" s="11"/>
     </row>
-    <row r="13" spans="1:29" ht="192" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:29" ht="192" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>520</v>
       </c>
@@ -4156,7 +4157,7 @@
       <c r="AB13" s="1"/>
       <c r="AC13" s="11"/>
     </row>
-    <row r="14" spans="1:29" ht="64" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:29" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>521</v>
       </c>
@@ -4217,7 +4218,7 @@
       <c r="AB14" s="1"/>
       <c r="AC14" s="11"/>
     </row>
-    <row r="15" spans="1:29" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:29" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>522</v>
       </c>
@@ -4280,7 +4281,7 @@
       <c r="AB15" s="1"/>
       <c r="AC15" s="11"/>
     </row>
-    <row r="16" spans="1:29" ht="192" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:29" ht="192" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>526</v>
       </c>
@@ -4343,7 +4344,7 @@
       <c r="AB16" s="1"/>
       <c r="AC16" s="11"/>
     </row>
-    <row r="17" spans="1:29" ht="96" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:29" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>527</v>
       </c>
@@ -4404,7 +4405,7 @@
       <c r="AB17" s="1"/>
       <c r="AC17" s="11"/>
     </row>
-    <row r="18" spans="1:29" ht="80" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:29" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>529</v>
       </c>
@@ -4469,7 +4470,7 @@
       <c r="AB18" s="1"/>
       <c r="AC18" s="11"/>
     </row>
-    <row r="19" spans="1:29" ht="96" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:29" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
         <v>564</v>
       </c>
@@ -4530,7 +4531,7 @@
       <c r="AB19" s="1"/>
       <c r="AC19" s="11"/>
     </row>
-    <row r="20" spans="1:29" ht="112" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:29" ht="112" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
         <v>565</v>
       </c>
@@ -4595,7 +4596,7 @@
       <c r="AB20" s="1"/>
       <c r="AC20" s="11"/>
     </row>
-    <row r="21" spans="1:29" ht="128" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:29" ht="128" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
         <v>566</v>
       </c>
@@ -4656,7 +4657,7 @@
       <c r="AB21" s="1"/>
       <c r="AC21" s="11"/>
     </row>
-    <row r="22" spans="1:29" ht="80" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:29" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
         <v>567</v>
       </c>
@@ -4717,7 +4718,7 @@
       <c r="AB22" s="1"/>
       <c r="AC22" s="11"/>
     </row>
-    <row r="23" spans="1:29" ht="176" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:29" ht="176" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
         <v>568</v>
       </c>
@@ -4778,7 +4779,7 @@
       <c r="AB23" s="1"/>
       <c r="AC23" s="11"/>
     </row>
-    <row r="24" spans="1:29" ht="144" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:29" ht="144" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
         <v>569</v>
       </c>
@@ -4841,7 +4842,7 @@
       <c r="AB24" s="1"/>
       <c r="AC24" s="11"/>
     </row>
-    <row r="25" spans="1:29" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:29" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
         <v>570</v>
       </c>
@@ -4902,7 +4903,7 @@
       <c r="AB25" s="1"/>
       <c r="AC25" s="11"/>
     </row>
-    <row r="26" spans="1:29" ht="288" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:29" ht="288" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
         <v>571</v>
       </c>
@@ -4969,7 +4970,7 @@
       <c r="AB26" s="1"/>
       <c r="AC26" s="11"/>
     </row>
-    <row r="27" spans="1:29" ht="128" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:29" ht="128" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
         <v>672</v>
       </c>
@@ -5032,7 +5033,7 @@
       <c r="AB27" s="1"/>
       <c r="AC27" s="11"/>
     </row>
-    <row r="28" spans="1:29" ht="112" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:29" ht="112" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
         <v>576</v>
       </c>
@@ -5093,7 +5094,7 @@
       <c r="AB28" s="1"/>
       <c r="AC28" s="11"/>
     </row>
-    <row r="29" spans="1:29" ht="128" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:29" ht="128" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
         <v>572</v>
       </c>
@@ -5156,7 +5157,7 @@
       <c r="AB29" s="1"/>
       <c r="AC29" s="11"/>
     </row>
-    <row r="30" spans="1:29" ht="128" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:29" ht="128" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
         <v>573</v>
       </c>
@@ -5219,7 +5220,7 @@
       <c r="AB30" s="1"/>
       <c r="AC30" s="11"/>
     </row>
-    <row r="31" spans="1:29" ht="144" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:29" ht="144" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
         <v>574</v>
       </c>
@@ -5284,7 +5285,7 @@
       <c r="AB31" s="1"/>
       <c r="AC31" s="11"/>
     </row>
-    <row r="32" spans="1:29" ht="112" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:29" ht="112" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
         <v>575</v>
       </c>
@@ -5345,7 +5346,7 @@
       <c r="AB32" s="1"/>
       <c r="AC32" s="11"/>
     </row>
-    <row r="33" spans="1:29" ht="192" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:29" ht="192" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>580</v>
       </c>
@@ -5406,7 +5407,7 @@
       <c r="AB33" s="1"/>
       <c r="AC33" s="11"/>
     </row>
-    <row r="34" spans="1:29" ht="128" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:29" ht="128" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>670</v>
       </c>
@@ -5469,7 +5470,7 @@
       <c r="AB34" s="1"/>
       <c r="AC34" s="11"/>
     </row>
-    <row r="35" spans="1:29" ht="208" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:29" ht="208" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>590</v>
       </c>
@@ -5532,7 +5533,7 @@
       <c r="AB35" s="1"/>
       <c r="AC35" s="11"/>
     </row>
-    <row r="36" spans="1:29" ht="48" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:29" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>644</v>
       </c>
@@ -5595,7 +5596,7 @@
       <c r="AB36" s="1"/>
       <c r="AC36" s="11"/>
     </row>
-    <row r="37" spans="1:29" ht="128" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:29" ht="128" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>589</v>
       </c>
@@ -5662,7 +5663,7 @@
       <c r="AB37" s="1"/>
       <c r="AC37" s="11"/>
     </row>
-    <row r="38" spans="1:29" ht="32" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:29" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>600</v>
       </c>
@@ -5729,7 +5730,7 @@
       <c r="AB38" s="1"/>
       <c r="AC38" s="11"/>
     </row>
-    <row r="39" spans="1:29" ht="48" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:29" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>598</v>
       </c>
@@ -5792,7 +5793,7 @@
       <c r="AB39" s="1"/>
       <c r="AC39" s="11"/>
     </row>
-    <row r="40" spans="1:29" ht="350" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:29" ht="350" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>599</v>
       </c>
@@ -5853,7 +5854,7 @@
       <c r="AB40" s="1"/>
       <c r="AC40" s="11"/>
     </row>
-    <row r="41" spans="1:29" ht="48" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:29" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>594</v>
       </c>
@@ -5914,7 +5915,7 @@
       <c r="AB41" s="1"/>
       <c r="AC41" s="11"/>
     </row>
-    <row r="42" spans="1:29" ht="112" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:29" ht="112" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>595</v>
       </c>
@@ -5981,7 +5982,7 @@
       <c r="AB42" s="1"/>
       <c r="AC42" s="11"/>
     </row>
-    <row r="43" spans="1:29" ht="64" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:29" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>596</v>
       </c>
@@ -6046,7 +6047,7 @@
       <c r="AB43" s="1"/>
       <c r="AC43" s="11"/>
     </row>
-    <row r="44" spans="1:29" ht="48" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:29" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>597</v>
       </c>
@@ -6115,7 +6116,7 @@
       <c r="AB44" s="1"/>
       <c r="AC44" s="11"/>
     </row>
-    <row r="45" spans="1:29" ht="64" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:29" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>584</v>
       </c>
@@ -6176,7 +6177,7 @@
       <c r="AB45" s="1"/>
       <c r="AC45" s="11"/>
     </row>
-    <row r="46" spans="1:29" ht="144" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:29" ht="144" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>591</v>
       </c>
@@ -6237,7 +6238,7 @@
       <c r="AB46" s="1"/>
       <c r="AC46" s="11"/>
     </row>
-    <row r="47" spans="1:29" ht="176" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:29" ht="176" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>592</v>
       </c>
@@ -6296,7 +6297,7 @@
       <c r="AB47" s="1"/>
       <c r="AC47" s="11"/>
     </row>
-    <row r="48" spans="1:29" ht="96" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:29" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>593</v>
       </c>
@@ -6798,7 +6799,7 @@
       <c r="AB55" s="1"/>
       <c r="AC55" s="11"/>
     </row>
-    <row r="56" spans="1:29" ht="80" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:29" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>505</v>
       </c>
@@ -6857,7 +6858,7 @@
       <c r="AB56" s="1"/>
       <c r="AC56" s="11"/>
     </row>
-    <row r="57" spans="1:29" ht="288" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:29" ht="288" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>511</v>
       </c>
@@ -6920,7 +6921,7 @@
       <c r="AB57" s="1"/>
       <c r="AC57" s="11"/>
     </row>
-    <row r="58" spans="1:29" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:29" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>510</v>
       </c>
@@ -6983,7 +6984,7 @@
       <c r="AB58" s="1"/>
       <c r="AC58" s="11"/>
     </row>
-    <row r="59" spans="1:29" ht="112" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:29" ht="112" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>513</v>
       </c>
@@ -7044,7 +7045,7 @@
       <c r="AB59" s="1"/>
       <c r="AC59" s="11"/>
     </row>
-    <row r="60" spans="1:29" ht="128" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:29" ht="128" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>512</v>
       </c>
@@ -7105,7 +7106,7 @@
       <c r="AB60" s="1"/>
       <c r="AC60" s="11"/>
     </row>
-    <row r="61" spans="1:29" ht="160" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:29" ht="160" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>509</v>
       </c>
@@ -7168,7 +7169,7 @@
       <c r="AB61" s="1"/>
       <c r="AC61" s="11"/>
     </row>
-    <row r="62" spans="1:29" ht="64" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:29" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>514</v>
       </c>
@@ -7229,7 +7230,7 @@
       <c r="AB62" s="1"/>
       <c r="AC62" s="11"/>
     </row>
-    <row r="63" spans="1:29" ht="64" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:29" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>515</v>
       </c>
@@ -7290,7 +7291,7 @@
       <c r="AB63" s="1"/>
       <c r="AC63" s="11"/>
     </row>
-    <row r="64" spans="1:29" ht="288" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:29" ht="288" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>516</v>
       </c>
@@ -7351,7 +7352,7 @@
       <c r="AB64" s="1"/>
       <c r="AC64" s="11"/>
     </row>
-    <row r="65" spans="1:29" ht="64" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:29" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>517</v>
       </c>
@@ -7412,7 +7413,7 @@
       <c r="AB65" s="1"/>
       <c r="AC65" s="11"/>
     </row>
-    <row r="66" spans="1:29" ht="256" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:29" ht="256" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>518</v>
       </c>
@@ -7475,7 +7476,7 @@
       <c r="AB66" s="1"/>
       <c r="AC66" s="11"/>
     </row>
-    <row r="67" spans="1:29" ht="96" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:29" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>525</v>
       </c>
@@ -7536,7 +7537,7 @@
       <c r="AB67" s="1"/>
       <c r="AC67" s="11"/>
     </row>
-    <row r="68" spans="1:29" ht="128" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:29" ht="128" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>523</v>
       </c>
@@ -7597,7 +7598,7 @@
       <c r="AB68" s="1"/>
       <c r="AC68" s="11"/>
     </row>
-    <row r="69" spans="1:29" ht="96" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:29" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>524</v>
       </c>
@@ -7662,7 +7663,7 @@
       <c r="AB69" s="1"/>
       <c r="AC69" s="11"/>
     </row>
-    <row r="70" spans="1:29" ht="160" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:29" ht="160" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>528</v>
       </c>
@@ -7727,7 +7728,7 @@
       <c r="AB70" s="1"/>
       <c r="AC70" s="11"/>
     </row>
-    <row r="71" spans="1:29" ht="112" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:29" ht="112" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>530</v>
       </c>
@@ -7788,7 +7789,7 @@
       <c r="AB71" s="1"/>
       <c r="AC71" s="11"/>
     </row>
-    <row r="72" spans="1:29" ht="96" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:29" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>531</v>
       </c>
@@ -7855,7 +7856,7 @@
       <c r="AB72" s="1"/>
       <c r="AC72" s="11"/>
     </row>
-    <row r="73" spans="1:29" ht="192" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:29" ht="192" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>532</v>
       </c>
@@ -7916,7 +7917,7 @@
       <c r="AB73" s="1"/>
       <c r="AC73" s="11"/>
     </row>
-    <row r="74" spans="1:29" ht="64" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:29" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="8" t="s">
         <v>535</v>
       </c>
@@ -7983,7 +7984,7 @@
       <c r="AB74" s="1"/>
       <c r="AC74" s="11"/>
     </row>
-    <row r="75" spans="1:29" ht="64" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:29" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="8" t="s">
         <v>536</v>
       </c>
@@ -8050,7 +8051,7 @@
       <c r="AB75" s="1"/>
       <c r="AC75" s="11"/>
     </row>
-    <row r="76" spans="1:29" ht="32" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:29" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="8" t="s">
         <v>537</v>
       </c>
@@ -8113,7 +8114,7 @@
       <c r="AB76" s="1"/>
       <c r="AC76" s="11"/>
     </row>
-    <row r="77" spans="1:29" ht="48" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:29" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="8" t="s">
         <v>538</v>
       </c>
@@ -8176,7 +8177,7 @@
       <c r="AB77" s="1"/>
       <c r="AC77" s="11"/>
     </row>
-    <row r="78" spans="1:29" ht="32" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:29" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="8" t="s">
         <v>539</v>
       </c>
@@ -8239,7 +8240,7 @@
       <c r="AB78" s="1"/>
       <c r="AC78" s="11"/>
     </row>
-    <row r="79" spans="1:29" ht="64" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:29" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="8" t="s">
         <v>540</v>
       </c>
@@ -8308,7 +8309,7 @@
       <c r="AB79" s="1"/>
       <c r="AC79" s="11"/>
     </row>
-    <row r="80" spans="1:29" ht="64" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:29" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="8" t="s">
         <v>541</v>
       </c>
@@ -8371,7 +8372,7 @@
       <c r="AB80" s="1"/>
       <c r="AC80" s="11"/>
     </row>
-    <row r="81" spans="1:29" ht="64" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:29" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="8" t="s">
         <v>542</v>
       </c>
@@ -8434,7 +8435,7 @@
       <c r="AB81" s="1"/>
       <c r="AC81" s="11"/>
     </row>
-    <row r="82" spans="1:29" ht="96" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:29" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="8" t="s">
         <v>533</v>
       </c>
@@ -8501,7 +8502,7 @@
       <c r="AB82" s="1"/>
       <c r="AC82" s="11"/>
     </row>
-    <row r="83" spans="1:29" ht="64" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:29" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="8" t="s">
         <v>534</v>
       </c>
@@ -8568,7 +8569,7 @@
       <c r="AB83" s="1"/>
       <c r="AC83" s="11"/>
     </row>
-    <row r="84" spans="1:29" ht="192" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:29" ht="192" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="8" t="s">
         <v>552</v>
       </c>
@@ -8631,7 +8632,7 @@
       <c r="AB84" s="1"/>
       <c r="AC84" s="11"/>
     </row>
-    <row r="85" spans="1:29" ht="208" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:29" ht="208" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="8" t="s">
         <v>553</v>
       </c>
@@ -8698,7 +8699,7 @@
       </c>
       <c r="AC85" s="11"/>
     </row>
-    <row r="86" spans="1:29" ht="96" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:29" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="8" t="s">
         <v>543</v>
       </c>
@@ -8759,7 +8760,7 @@
       <c r="AB86" s="1"/>
       <c r="AC86" s="11"/>
     </row>
-    <row r="87" spans="1:29" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:29" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="8" t="s">
         <v>554</v>
       </c>
@@ -8820,7 +8821,7 @@
       <c r="AB87" s="1"/>
       <c r="AC87" s="11"/>
     </row>
-    <row r="88" spans="1:29" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:29" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="8" t="s">
         <v>555</v>
       </c>
@@ -8881,7 +8882,7 @@
       <c r="AB88" s="1"/>
       <c r="AC88" s="11"/>
     </row>
-    <row r="89" spans="1:29" ht="96" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:29" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="8" t="s">
         <v>544</v>
       </c>
@@ -8942,7 +8943,7 @@
       <c r="AB89" s="1"/>
       <c r="AC89" s="11"/>
     </row>
-    <row r="90" spans="1:29" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:29" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="8" t="s">
         <v>556</v>
       </c>
@@ -9005,7 +9006,7 @@
       <c r="AB90" s="1"/>
       <c r="AC90" s="11"/>
     </row>
-    <row r="91" spans="1:29" ht="160" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:29" ht="160" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="8" t="s">
         <v>557</v>
       </c>
@@ -9066,7 +9067,7 @@
       <c r="AB91" s="1"/>
       <c r="AC91" s="11"/>
     </row>
-    <row r="92" spans="1:29" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:29" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="8" t="s">
         <v>558</v>
       </c>
@@ -9131,7 +9132,7 @@
       <c r="AB92" s="1"/>
       <c r="AC92" s="11"/>
     </row>
-    <row r="93" spans="1:29" ht="64" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:29" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" s="8" t="s">
         <v>545</v>
       </c>
@@ -9192,7 +9193,7 @@
       <c r="AB93" s="1"/>
       <c r="AC93" s="11"/>
     </row>
-    <row r="94" spans="1:29" ht="208" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:29" ht="208" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="8" t="s">
         <v>559</v>
       </c>
@@ -9253,7 +9254,7 @@
       <c r="AB94" s="1"/>
       <c r="AC94" s="11"/>
     </row>
-    <row r="95" spans="1:29" ht="64" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:29" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="8" t="s">
         <v>546</v>
       </c>
@@ -9314,7 +9315,7 @@
       <c r="AB95" s="1"/>
       <c r="AC95" s="11"/>
     </row>
-    <row r="96" spans="1:29" ht="350" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:29" ht="350" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="8" t="s">
         <v>560</v>
       </c>
@@ -9381,7 +9382,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="97" spans="1:29" ht="128" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:29" ht="128" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="8" t="s">
         <v>561</v>
       </c>
@@ -9442,7 +9443,7 @@
       <c r="AB97" s="1"/>
       <c r="AC97" s="11"/>
     </row>
-    <row r="98" spans="1:29" ht="129" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:29" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A98" s="8" t="s">
         <v>562</v>
       </c>
@@ -9501,7 +9502,7 @@
       <c r="AB98" s="1"/>
       <c r="AC98" s="11"/>
     </row>
-    <row r="99" spans="1:29" ht="128" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:29" ht="128" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="8" t="s">
         <v>563</v>
       </c>
@@ -9562,7 +9563,7 @@
       <c r="AB99" s="1"/>
       <c r="AC99" s="11"/>
     </row>
-    <row r="100" spans="1:29" ht="96" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:29" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="8" t="s">
         <v>547</v>
       </c>
@@ -9623,7 +9624,7 @@
       <c r="AB100" s="1"/>
       <c r="AC100" s="11"/>
     </row>
-    <row r="101" spans="1:29" ht="64" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:29" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="8" t="s">
         <v>548</v>
       </c>
@@ -9684,7 +9685,7 @@
       <c r="AB101" s="1"/>
       <c r="AC101" s="11"/>
     </row>
-    <row r="102" spans="1:29" ht="64" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:29" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="8" t="s">
         <v>549</v>
       </c>
@@ -9745,7 +9746,7 @@
       <c r="AB102" s="1"/>
       <c r="AC102" s="11"/>
     </row>
-    <row r="103" spans="1:29" ht="80" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:29" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="8" t="s">
         <v>550</v>
       </c>
@@ -9806,7 +9807,7 @@
       <c r="AB103" s="1"/>
       <c r="AC103" s="11"/>
     </row>
-    <row r="104" spans="1:29" ht="80" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:29" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="8" t="s">
         <v>551</v>
       </c>
@@ -9869,7 +9870,7 @@
       <c r="AB104" s="1"/>
       <c r="AC104" s="11"/>
     </row>
-    <row r="105" spans="1:29" ht="176" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:29" ht="176" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>578</v>
       </c>
@@ -9934,7 +9935,7 @@
       <c r="AB105" s="1"/>
       <c r="AC105" s="11"/>
     </row>
-    <row r="106" spans="1:29" ht="365" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:29" ht="365" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>577</v>
       </c>
@@ -10001,7 +10002,7 @@
       <c r="AB106" s="1"/>
       <c r="AC106" s="11"/>
     </row>
-    <row r="107" spans="1:29" ht="80" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:29" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>579</v>
       </c>
@@ -10066,7 +10067,7 @@
       <c r="AB107" s="1"/>
       <c r="AC107" s="11"/>
     </row>
-    <row r="108" spans="1:29" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:29" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>583</v>
       </c>
@@ -10141,7 +10142,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="109" spans="1:29" ht="64" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:29" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>633</v>
       </c>
@@ -10210,7 +10211,7 @@
       <c r="AB109" s="1"/>
       <c r="AC109" s="11"/>
     </row>
-    <row r="110" spans="1:29" ht="144" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:29" ht="144" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>634</v>
       </c>
@@ -10289,7 +10290,7 @@
       </c>
       <c r="AC110" s="11"/>
     </row>
-    <row r="111" spans="1:29" ht="64" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:29" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>635</v>
       </c>
@@ -10352,7 +10353,7 @@
       <c r="AB111" s="1"/>
       <c r="AC111" s="11"/>
     </row>
-    <row r="112" spans="1:29" ht="160" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:29" ht="160" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>636</v>
       </c>
@@ -10419,7 +10420,7 @@
       </c>
       <c r="AC112" s="11"/>
     </row>
-    <row r="113" spans="1:29" ht="365" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:29" ht="365" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>588</v>
       </c>
@@ -10488,7 +10489,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="114" spans="1:29" ht="320" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:29" ht="320" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>581</v>
       </c>
@@ -10551,7 +10552,7 @@
       <c r="AB114" s="1"/>
       <c r="AC114" s="11"/>
     </row>
-    <row r="115" spans="1:29" ht="409.6" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:29" ht="409.6" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>582</v>
       </c>
@@ -10618,7 +10619,7 @@
       <c r="AB115" s="1"/>
       <c r="AC115" s="11"/>
     </row>
-    <row r="116" spans="1:29" ht="48" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:29" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>587</v>
       </c>
@@ -10683,7 +10684,7 @@
       <c r="AB116" s="1"/>
       <c r="AC116" s="11"/>
     </row>
-    <row r="117" spans="1:29" ht="288" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:29" ht="288" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>586</v>
       </c>
@@ -10752,7 +10753,7 @@
       <c r="AB117" s="1"/>
       <c r="AC117" s="11"/>
     </row>
-    <row r="118" spans="1:29" ht="396" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:29" ht="396" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>585</v>
       </c>
@@ -10821,6 +10822,16 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:AC118" xr:uid="{B84DAE8B-405E-4655-89DF-BEE99C6D5E84}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="ERA, Vene"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="2">
+      <filters>
+        <filter val="1"/>
+      </filters>
+    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AC118">
       <sortCondition ref="R1:R118"/>
     </sortState>

</xml_diff>